<commit_message>
Clean up: Remove unused test files, old reports, temp artifacts, and obsolete helpers
</commit_message>
<xml_diff>
--- a/WB_Test_Report_2025-12-22.xlsx
+++ b/WB_Test_Report_2025-12-22.xlsx
@@ -4,11 +4,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="BOP_1" sheetId="2" r:id="rId2"/>
-    <sheet name="BOP_2" sheetId="3" r:id="rId3"/>
-    <sheet name="BOP_3" sheetId="4" r:id="rId4"/>
-    <sheet name="BOP_4" sheetId="5" r:id="rId5"/>
-    <sheet name="BOP_5" sheetId="6" r:id="rId6"/>
+    <sheet name="Package_1" sheetId="2" r:id="rId2"/>
+    <sheet name="Package_2" sheetId="3" r:id="rId3"/>
+    <sheet name="Package_3" sheetId="4" r:id="rId4"/>
+    <sheet name="Package_4" sheetId="5" r:id="rId5"/>
+    <sheet name="Package_5" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -435,7 +435,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>BOP</v>
+        <v>Package</v>
       </c>
       <c r="C2" t="str">
         <v>N/A</v>
@@ -458,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>BOP</v>
+        <v>Package</v>
       </c>
       <c r="C3" t="str">
         <v>N/A</v>
@@ -470,10 +470,10 @@
         <v>FAILED</v>
       </c>
       <c r="F3" t="str">
-        <v>83.67</v>
+        <v>187.95</v>
       </c>
       <c r="G3" t="str">
-        <v>WI</v>
+        <v>PA</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>BOP</v>
+        <v>Package</v>
       </c>
       <c r="C4" t="str">
         <v>N/A</v>
@@ -493,7 +493,7 @@
         <v>FAILED</v>
       </c>
       <c r="F4" t="str">
-        <v>251.13</v>
+        <v>187.95</v>
       </c>
       <c r="G4" t="str">
         <v>PA</v>
@@ -504,22 +504,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>BOP</v>
+        <v>Package</v>
       </c>
       <c r="C5" t="str">
-        <v>3003179089</v>
+        <v>N/A</v>
       </c>
       <c r="D5" t="str">
-        <v>1003052683</v>
+        <v>N/A</v>
       </c>
       <c r="E5" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="F5" t="str">
-        <v>480.36</v>
+        <v>236.86</v>
       </c>
       <c r="G5" t="str">
-        <v>MI</v>
+        <v>DE</v>
       </c>
     </row>
     <row r="6">
@@ -527,22 +527,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>BOP</v>
+        <v>Package</v>
       </c>
       <c r="C6" t="str">
-        <v>3003179093</v>
+        <v>3003179091</v>
       </c>
       <c r="D6" t="str">
-        <v>1003052684</v>
+        <v>1003052685</v>
       </c>
       <c r="E6" t="str">
         <v>PASSED</v>
       </c>
       <c r="F6" t="str">
-        <v>499.27</v>
+        <v>823.69</v>
       </c>
       <c r="G6" t="str">
-        <v>PA</v>
+        <v>WI</v>
       </c>
     </row>
   </sheetData>
@@ -596,7 +596,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -617,21 +617,35 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>Account Created</v>
+      </c>
+      <c r="B2" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C2" t="str">
+        <v>106.45s</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-12-22T01:37:33.339Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
         <v>Test Execution Failed</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B3" t="str">
         <v>FAILED</v>
       </c>
-      <c r="C2" t="str">
-        <v>83.67s</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2025-12-22T01:37:10.514Z</v>
+      <c r="C3" t="str">
+        <v>81.50s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-22T01:38:54.844Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -665,24 +679,24 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>105.43s</v>
+        <v>106.45s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-22T01:37:32.279Z</v>
+        <v>2025-12-22T01:37:33.339Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Building and Classification Added</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>145.70s</v>
+        <v>81.50s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-22T01:39:57.983Z</v>
+        <v>2025-12-22T01:38:54.844Z</v>
       </c>
     </row>
   </sheetData>
@@ -694,7 +708,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -721,92 +735,36 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>97.94s</v>
+        <v>95.32s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-22T01:37:25.006Z</v>
+        <v>2025-12-22T01:37:22.073Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Building and Classification Added</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>143.51s</v>
+        <v>141.54s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-22T01:39:48.519Z</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
-      </c>
-      <c r="B4" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C4" t="str">
-        <v>20.48s</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2025-12-22T01:40:08.996Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C5" t="str">
-        <v>0.03s</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2025-12-22T01:40:09.030Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>UW Issues Approved</v>
-      </c>
-      <c r="B6" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C6" t="str">
-        <v>218.40s</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2025-12-22T01:43:47.433Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Policy Issued Successfully</v>
-      </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
-        <v>0.00s</v>
-      </c>
-      <c r="D7" t="str">
-        <v>2025-12-22T01:43:47.435Z</v>
+        <v>2025-12-22T01:39:43.611Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -833,85 +791,127 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>105.43s</v>
+        <v>103.40s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-22T01:37:32.279Z</v>
+        <v>2025-12-22T01:37:30.231Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Building and Classification Added</v>
+        <v>Commercial Property Package Completed</v>
       </c>
       <c r="B3" t="str">
         <v>PASSED</v>
       </c>
       <c r="C3" t="str">
-        <v>145.70s</v>
+        <v>286.56s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-22T01:39:57.983Z</v>
+        <v>2025-12-22T01:42:16.794Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
+        <v>General Liability Completed</v>
       </c>
       <c r="B4" t="str">
         <v>PASSED</v>
       </c>
       <c r="C4" t="str">
-        <v>22.36s</v>
+        <v>81.66s</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-12-22T01:40:20.347Z</v>
+        <v>2025-12-22T01:43:38.453Z</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Submitting for Approval</v>
+        <v>Inland Marine Completed</v>
       </c>
       <c r="B5" t="str">
         <v>PASSED</v>
       </c>
       <c r="C5" t="str">
-        <v>0.00s</v>
+        <v>35.45s</v>
       </c>
       <c r="D5" t="str">
-        <v>2025-12-22T01:40:20.353Z</v>
+        <v>2025-12-22T01:44:13.904Z</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>UW Issues Approved</v>
+        <v>Crime Completed</v>
       </c>
       <c r="B6" t="str">
         <v>PASSED</v>
       </c>
       <c r="C6" t="str">
-        <v>225.78s</v>
+        <v>22.85s</v>
       </c>
       <c r="D6" t="str">
-        <v>2025-12-22T01:44:06.135Z</v>
+        <v>2025-12-22T01:44:39.812Z</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>60.26s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-22T01:45:40.076Z</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B8" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C8" t="str">
+        <v>0.00s</v>
+      </c>
+      <c r="D8" t="str">
+        <v>2025-12-22T01:45:40.082Z</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>UW Issues Approved</v>
+      </c>
+      <c r="B9" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C9" t="str">
+        <v>233.51s</v>
+      </c>
+      <c r="D9" t="str">
+        <v>2025-12-22T01:49:33.589Z</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
         <v>Policy Issued Successfully</v>
       </c>
-      <c r="B7" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C7" t="str">
+      <c r="B10" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C10" t="str">
         <v>0.00s</v>
       </c>
-      <c r="D7" t="str">
-        <v>2025-12-22T01:44:06.137Z</v>
+      <c r="D10" t="str">
+        <v>2025-12-22T01:49:33.592Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(email): send partial email on interrupted batch; grace wait then fallback to available suites
</commit_message>
<xml_diff>
--- a/WB_Test_Report_2025-12-22.xlsx
+++ b/WB_Test_Report_2025-12-22.xlsx
@@ -4,7 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="BOP_1" sheetId="2" r:id="rId2"/>
+    <sheet name="BOP_16" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -425,13 +425,13 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B2" t="str">
-        <v>BOP (DE)</v>
+        <v>BOP (OH)</v>
       </c>
       <c r="C2" t="str">
-        <v>3003179162</v>
+        <v>N/A</v>
       </c>
       <c r="D2" t="str">
         <v>N/A</v>
@@ -440,7 +440,7 @@
         <v>FAILED</v>
       </c>
       <c r="F2" t="str">
-        <v>342.79</v>
+        <v>228.42</v>
       </c>
     </row>
   </sheetData>
@@ -452,7 +452,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -479,10 +479,10 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>96.36s</v>
+        <v>84.67s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-22T14:18:36.645Z</v>
+        <v>2025-12-22T14:51:40.324Z</v>
       </c>
     </row>
     <row r="3">
@@ -493,57 +493,29 @@
         <v>PASSED</v>
       </c>
       <c r="C3" t="str">
-        <v>134.78s</v>
+        <v>138.63s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-22T14:20:51.424Z</v>
+        <v>2025-12-22T14:53:58.960Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Quote Rated Successfully</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B4" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C4" t="str">
-        <v>22.11s</v>
+        <v>5.12s</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-12-22T14:21:13.541Z</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Submitting for Approval</v>
-      </c>
-      <c r="B5" t="str">
-        <v>PASSED</v>
-      </c>
-      <c r="C5" t="str">
-        <v>0.04s</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2025-12-22T14:21:20.518Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Test Execution Failed</v>
-      </c>
-      <c r="B6" t="str">
-        <v>FAILED</v>
-      </c>
-      <c r="C6" t="str">
-        <v>89.50s</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2025-12-22T14:22:50.029Z</v>
+        <v>2025-12-22T14:54:04.077Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix email consolidation: stop per-iteration emails, ensure suite-specific sends, clean cross-suite iterations
</commit_message>
<xml_diff>
--- a/WB_Test_Report_2025-12-22.xlsx
+++ b/WB_Test_Report_2025-12-22.xlsx
@@ -4,7 +4,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="BOP_16" sheetId="2" r:id="rId2"/>
+    <sheet name="Package_1" sheetId="2" r:id="rId2"/>
+    <sheet name="Package_2" sheetId="3" r:id="rId3"/>
+    <sheet name="Package_3" sheetId="4" r:id="rId4"/>
+    <sheet name="Package_4" sheetId="5" r:id="rId5"/>
+    <sheet name="Package_5" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -398,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,16 +426,19 @@
       <c r="F1" t="str">
         <v>Duration (s)</v>
       </c>
+      <c r="G1" t="str">
+        <v>State</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>BOP (OH)</v>
+        <v>Package (WI)</v>
       </c>
       <c r="C2" t="str">
-        <v>N/A</v>
+        <v>3003179292</v>
       </c>
       <c r="D2" t="str">
         <v>N/A</v>
@@ -440,19 +447,114 @@
         <v>FAILED</v>
       </c>
       <c r="F2" t="str">
-        <v>228.42</v>
+        <v>164.08</v>
+      </c>
+      <c r="G2" t="str">
+        <v>WI</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Package (PA)</v>
+      </c>
+      <c r="C3" t="str">
+        <v>3003179291</v>
+      </c>
+      <c r="D3" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="E3" t="str">
+        <v>FAILED</v>
+      </c>
+      <c r="F3" t="str">
+        <v>327.67</v>
+      </c>
+      <c r="G3" t="str">
+        <v>PA</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Package (DE)</v>
+      </c>
+      <c r="C4" t="str">
+        <v>3003179293</v>
+      </c>
+      <c r="D4" t="str">
+        <v>1003052717</v>
+      </c>
+      <c r="E4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="F4" t="str">
+        <v>825.68</v>
+      </c>
+      <c r="G4" t="str">
+        <v>DE</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Package (OH)</v>
+      </c>
+      <c r="C5" t="str">
+        <v>3003179299</v>
+      </c>
+      <c r="D5" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="E5" t="str">
+        <v>FAILED</v>
+      </c>
+      <c r="F5" t="str">
+        <v>151.36</v>
+      </c>
+      <c r="G5" t="str">
+        <v>OH</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Package (MI)</v>
+      </c>
+      <c r="C6" t="str">
+        <v>3003179298</v>
+      </c>
+      <c r="D6" t="str">
+        <v>1003052718</v>
+      </c>
+      <c r="E6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="F6" t="str">
+        <v>777.45</v>
+      </c>
+      <c r="G6" t="str">
+        <v>MI</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -479,43 +581,449 @@
         <v>PASSED</v>
       </c>
       <c r="C2" t="str">
-        <v>84.67s</v>
+        <v>87.59s</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-12-22T14:51:40.324Z</v>
+        <v>2025-12-22T20:47:05.256Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Building and Classification Added</v>
+        <v>Test Execution Failed</v>
       </c>
       <c r="B3" t="str">
-        <v>PASSED</v>
+        <v>FAILED</v>
       </c>
       <c r="C3" t="str">
-        <v>138.63s</v>
+        <v>76.49s</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-12-22T14:53:58.960Z</v>
+        <v>2025-12-22T20:48:21.749Z</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Milestone</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Duration (s)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Timestamp</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Account Created</v>
+      </c>
+      <c r="B2" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C2" t="str">
+        <v>78.14s</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-12-22T20:46:54.089Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Test Execution Failed</v>
+      </c>
+      <c r="B3" t="str">
+        <v>FAILED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>249.53s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-22T20:51:03.626Z</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Milestone</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Duration (s)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Timestamp</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Account Created</v>
+      </c>
+      <c r="B2" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C2" t="str">
+        <v>99.75s</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-12-22T20:47:14.474Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Commercial Property Package Completed</v>
+      </c>
+      <c r="B3" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>278.46s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-22T20:51:52.938Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Test Execution Failed</v>
+        <v>General Liability Completed</v>
       </c>
       <c r="B4" t="str">
-        <v>FAILED</v>
+        <v>PASSED</v>
       </c>
       <c r="C4" t="str">
-        <v>5.12s</v>
+        <v>79.58s</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-12-22T14:54:04.077Z</v>
+        <v>2025-12-22T20:53:12.523Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Inland Marine Completed</v>
+      </c>
+      <c r="B5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C5" t="str">
+        <v>35.14s</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-22T20:53:47.669Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Crime Completed</v>
+      </c>
+      <c r="B6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C6" t="str">
+        <v>23.02s</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-12-22T20:54:10.691Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>60.25s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-22T20:55:10.940Z</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B8" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C8" t="str">
+        <v>32.17s</v>
+      </c>
+      <c r="D8" t="str">
+        <v>2025-12-22T20:55:43.116Z</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B9" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C9" t="str">
+        <v>63.81s</v>
+      </c>
+      <c r="D9" t="str">
+        <v>2025-12-22T20:56:46.931Z</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Policy Issued Successfully</v>
+      </c>
+      <c r="B10" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C10" t="str">
+        <v>153.50s</v>
+      </c>
+      <c r="D10" t="str">
+        <v>2025-12-22T20:59:20.436Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Milestone</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Duration (s)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Timestamp</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Account Created</v>
+      </c>
+      <c r="B2" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C2" t="str">
+        <v>84.51s</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-12-22T21:00:42.639Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Test Execution Failed</v>
+      </c>
+      <c r="B3" t="str">
+        <v>FAILED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>66.85s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-22T21:01:49.500Z</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Milestone</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Duration (s)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Timestamp</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Account Created</v>
+      </c>
+      <c r="B2" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C2" t="str">
+        <v>83.03s</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2025-12-22T21:00:41.569Z</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Commercial Property Package Completed</v>
+      </c>
+      <c r="B3" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C3" t="str">
+        <v>271.39s</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-22T21:05:12.969Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>General Liability Completed</v>
+      </c>
+      <c r="B4" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C4" t="str">
+        <v>75.41s</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2025-12-22T21:06:28.378Z</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Inland Marine Completed</v>
+      </c>
+      <c r="B5" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C5" t="str">
+        <v>34.87s</v>
+      </c>
+      <c r="D5" t="str">
+        <v>2025-12-22T21:07:03.247Z</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Crime Completed</v>
+      </c>
+      <c r="B6" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C6" t="str">
+        <v>22.03s</v>
+      </c>
+      <c r="D6" t="str">
+        <v>2025-12-22T21:07:25.285Z</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Quote Rated Successfully</v>
+      </c>
+      <c r="B7" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C7" t="str">
+        <v>60.24s</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-22T21:08:25.531Z</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Submitting for Approval</v>
+      </c>
+      <c r="B8" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C8" t="str">
+        <v>33.16s</v>
+      </c>
+      <c r="D8" t="str">
+        <v>2025-12-22T21:08:58.690Z</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>UW Issues Approved in PolicyCenter</v>
+      </c>
+      <c r="B9" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C9" t="str">
+        <v>45.54s</v>
+      </c>
+      <c r="D9" t="str">
+        <v>2025-12-22T21:09:44.232Z</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Policy Issued Successfully</v>
+      </c>
+      <c r="B10" t="str">
+        <v>PASSED</v>
+      </c>
+      <c r="C10" t="str">
+        <v>151.78s</v>
+      </c>
+      <c r="D10" t="str">
+        <v>2025-12-22T21:12:16.015Z</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>